<commit_message>
Most recent model version, updated covid recession
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -175,19 +175,19 @@
     <t>Table 9a</t>
   </si>
   <si>
-    <t>As of EPS 2.1.1, this variable is set up to model the impacts of the 2020</t>
-  </si>
-  <si>
     <t>Real GDP (billion chained 2012 dollars)</t>
   </si>
   <si>
-    <t>September STEO</t>
-  </si>
-  <si>
-    <t>January 2020 and September 2020</t>
-  </si>
-  <si>
-    <t>SARS-CoV-2 pandemic.  It uses the latest data available as of September 9,</t>
+    <t>November STEO</t>
+  </si>
+  <si>
+    <t>January 2020 and November 2020</t>
+  </si>
+  <si>
+    <t>As of EPS 3.1, this variable is set up to model the impacts of the 2020</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2 pandemic.  It uses the latest data available as of November 10,</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -716,7 +716,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
@@ -804,7 +804,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -817,7 +817,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -848,16 +848,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3">
-        <v>19073</v>
+        <v>19092</v>
       </c>
       <c r="C3">
-        <v>18168</v>
+        <v>18411</v>
       </c>
       <c r="D3">
-        <v>18726</v>
+        <v>19098</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -892,15 +892,15 @@
       </c>
       <c r="B5">
         <f>B3</f>
-        <v>19073</v>
+        <v>19092</v>
       </c>
       <c r="C5" s="20">
         <f>C4*($B$3/$B$4)</f>
-        <v>19453.099643381582</v>
+        <v>19472.478288231592</v>
       </c>
       <c r="D5" s="20">
         <f>D4*($B$3/$B$4)</f>
-        <v>19795.189322425005</v>
+        <v>19814.908747640027</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -935,11 +935,11 @@
       </c>
       <c r="C8" s="5">
         <f>(C3-C5)/C5</f>
-        <v>-6.6061433238933931E-2</v>
+        <v>-5.4511720209394626E-2</v>
       </c>
       <c r="D8" s="5">
         <f>(D3-D5)/D5</f>
-        <v>-5.4012583815693682E-2</v>
+        <v>-3.6180269955843815E-2</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
@@ -991,7 +991,7 @@
       </c>
       <c r="B12" s="12">
         <f>C3/B3-1</f>
-        <v>-4.7449273842604778E-2</v>
+        <v>-3.5669390320553163E-2</v>
       </c>
       <c r="C12" s="15"/>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B2" s="22">
         <f>Data!B12</f>
-        <v>-4.7449273842604778E-2</v>
+        <v>-3.5669390320553163E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>